<commit_message>
finish day 4, add references
</commit_message>
<xml_diff>
--- a/课表.xlsx
+++ b/课表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\上课\软件工程营\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\上课\软件工程营\2023\Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>下午</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,13 +86,16 @@
   </si>
   <si>
     <t>Household Electric Power Consumption</t>
+  </si>
+  <si>
+    <t>上课时间地点：上午8：30，下午14：30，地点=电气大楼B305</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,8 +111,24 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +141,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -132,12 +156,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -150,8 +175,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="差" xfId="1" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,7 +462,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -445,86 +474,80 @@
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" ht="23.4">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="49.95" customHeight="1">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="49.95" customHeight="1">
-      <c r="A2" s="1">
-        <v>45152</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="49.95" customHeight="1">
       <c r="A3" s="1">
-        <v>45153</v>
+        <v>45152</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="49.95" customHeight="1">
       <c r="A4" s="1">
-        <v>45154</v>
+        <v>45153</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="49.95" customHeight="1">
       <c r="A5" s="1">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="49.95" customHeight="1">
       <c r="A6" s="1">
-        <v>45156</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>45155</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -533,7 +556,7 @@
     </row>
     <row r="7" spans="1:5" ht="49.95" customHeight="1">
       <c r="A7" s="1">
-        <v>45157</v>
+        <v>45156</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -548,7 +571,7 @@
     </row>
     <row r="8" spans="1:5" ht="49.95" customHeight="1">
       <c r="A8" s="1">
-        <v>45158</v>
+        <v>45157</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
@@ -563,13 +586,13 @@
     </row>
     <row r="9" spans="1:5" ht="49.95" customHeight="1">
       <c r="A9" s="1">
-        <v>45159</v>
+        <v>45158</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>
@@ -578,13 +601,13 @@
     </row>
     <row r="10" spans="1:5" ht="49.95" customHeight="1">
       <c r="A10" s="1">
-        <v>45160</v>
+        <v>45159</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>5</v>
@@ -593,13 +616,13 @@
     </row>
     <row r="11" spans="1:5" ht="49.95" customHeight="1">
       <c r="A11" s="1">
-        <v>45161</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>6</v>
+        <v>45160</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>5</v>
@@ -608,13 +631,13 @@
     </row>
     <row r="12" spans="1:5" ht="49.95" customHeight="1">
       <c r="A12" s="1">
-        <v>45162</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>45161</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
@@ -623,7 +646,7 @@
     </row>
     <row r="13" spans="1:5" ht="49.95" customHeight="1">
       <c r="A13" s="1">
-        <v>45163</v>
+        <v>45162</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
@@ -638,21 +661,29 @@
     </row>
     <row r="14" spans="1:5" ht="49.95" customHeight="1">
       <c r="A14" s="1">
+        <v>45163</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="49.95" customHeight="1">
+      <c r="A15" s="1">
         <v>45164</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" ht="49.95" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -699,6 +730,9 @@
       <c r="E21" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>